<commit_message>
some fixes/changes to performance models and more measurements
</commit_message>
<xml_diff>
--- a/Measurements.xlsx
+++ b/Measurements.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Problem: 1600x1600x30s augRieSolver</t>
   </si>
@@ -28,18 +28,33 @@
     <t xml:space="preserve">sec</t>
   </si>
   <si>
+    <t xml:space="preserve">Problem; 2512x2512 augRie, radial Dam break</t>
+  </si>
+  <si>
     <t xml:space="preserve">CPU ONLY</t>
   </si>
   <si>
+    <t xml:space="preserve">Single-node CPU</t>
+  </si>
+  <si>
     <t xml:space="preserve">GPU ONLY</t>
   </si>
   <si>
+    <t xml:space="preserve">Single-node CUDA</t>
+  </si>
+  <si>
     <t xml:space="preserve">CPU_MPI</t>
   </si>
   <si>
+    <t xml:space="preserve">MPI CPU</t>
+  </si>
+  <si>
     <t xml:space="preserve">STARPU_EAGER</t>
   </si>
   <si>
+    <t xml:space="preserve">MPI CUDA</t>
+  </si>
+  <si>
     <t xml:space="preserve">STARPU_RANDOM</t>
   </si>
   <si>
@@ -49,6 +64,9 @@
     <t xml:space="preserve">STARPU_LOCAL_WORK_STEALING</t>
   </si>
   <si>
+    <t xml:space="preserve">STARPU_LOCAL_WORK_STEALING 2x2</t>
+  </si>
+  <si>
     <t xml:space="preserve">STARPU_HETEROPRIO</t>
   </si>
   <si>
@@ -61,7 +79,13 @@
     <t xml:space="preserve">dm</t>
   </si>
   <si>
+    <t xml:space="preserve">dm 2x2</t>
+  </si>
+  <si>
     <t xml:space="preserve">dmdap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dmda 2x2</t>
   </si>
 </sst>
 </file>
@@ -162,16 +186,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="37.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.9"/>
@@ -184,67 +208,100 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>88</v>
       </c>
+      <c r="E4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>345</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="E5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>46</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="E6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>465</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>78</v>
       </c>
+      <c r="E10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>677</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>7</v>
@@ -252,18 +309,30 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="E15" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>7</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>